<commit_message>
update script for file path change
</commit_message>
<xml_diff>
--- a/Readme/controller_win.xlsx
+++ b/Readme/controller_win.xlsx
@@ -530,7 +530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -574,11 +576,11 @@
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
@@ -599,11 +601,11 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1">
@@ -700,11 +702,11 @@
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>13</v>

</xml_diff>